<commit_message>
spreadsheet generated for midterm
</commit_message>
<xml_diff>
--- a/hw4/flower/generated_spreadsheet.xlsx
+++ b/hw4/flower/generated_spreadsheet.xlsx
@@ -1734,7 +1734,7 @@
         <v>98</v>
       </c>
       <c r="C3">
-        <v>129.5</v>
+        <v>131.25</v>
       </c>
       <c r="D3">
         <v>133</v>
@@ -1769,28 +1769,28 @@
         <v>106</v>
       </c>
       <c r="C4">
-        <v>127.15</v>
+        <v>129.9875</v>
       </c>
       <c r="D4">
-        <v>129.5</v>
+        <v>131.25</v>
       </c>
       <c r="E4">
-        <v>23.5</v>
+        <v>25.25</v>
       </c>
       <c r="F4">
-        <v>23.5</v>
+        <v>25.25</v>
       </c>
       <c r="G4">
-        <v>888.625</v>
+        <v>931.28125</v>
       </c>
       <c r="H4">
-        <v>29.25</v>
+        <v>30.125</v>
       </c>
       <c r="I4">
-        <v>22.16981132075472</v>
+        <v>23.82075471698113</v>
       </c>
       <c r="J4">
-        <v>28.94204851752022</v>
+        <v>29.76752021563343</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -1804,28 +1804,28 @@
         <v>109</v>
       </c>
       <c r="C5">
-        <v>125.335</v>
+        <v>128.938125</v>
       </c>
       <c r="D5">
-        <v>127.15</v>
+        <v>129.9875</v>
       </c>
       <c r="E5">
-        <v>18.15000000000001</v>
+        <v>20.98750000000001</v>
       </c>
       <c r="F5">
-        <v>18.15000000000001</v>
+        <v>20.98750000000001</v>
       </c>
       <c r="G5">
-        <v>702.2241666666667</v>
+        <v>767.6792187500001</v>
       </c>
       <c r="H5">
-        <v>25.55</v>
+        <v>27.07916666666667</v>
       </c>
       <c r="I5">
-        <v>16.65137614678899</v>
+        <v>19.25458715596331</v>
       </c>
       <c r="J5">
-        <v>24.84515772727648</v>
+        <v>26.26320919574339</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -1839,31 +1839,31 @@
         <v>133</v>
       </c>
       <c r="C6">
-        <v>126.1015</v>
+        <v>129.14121875</v>
       </c>
       <c r="D6">
-        <v>125.335</v>
+        <v>128.938125</v>
       </c>
       <c r="E6">
-        <v>-7.664999999999992</v>
+        <v>-4.061874999999986</v>
       </c>
       <c r="F6">
-        <v>7.664999999999992</v>
+        <v>4.061874999999986</v>
       </c>
       <c r="G6">
-        <v>541.35618125</v>
+        <v>579.8841211914064</v>
       </c>
       <c r="H6">
-        <v>21.07875</v>
+        <v>21.32484375</v>
       </c>
       <c r="I6">
-        <v>5.763157894736836</v>
+        <v>3.054041353383448</v>
       </c>
       <c r="J6">
-        <v>20.07465776914157</v>
+        <v>20.46091723515341</v>
       </c>
       <c r="K6">
-        <v>3.272727272727273</v>
+        <v>3.61904761904762</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1874,31 +1874,31 @@
         <v>130</v>
       </c>
       <c r="C7">
-        <v>126.49135</v>
+        <v>129.1841578125</v>
       </c>
       <c r="D7">
-        <v>126.1015</v>
+        <v>129.14121875</v>
       </c>
       <c r="E7">
-        <v>-3.898499999999999</v>
+        <v>-0.8587812499999927</v>
       </c>
       <c r="F7">
-        <v>3.898499999999999</v>
+        <v>0.8587812499999927</v>
       </c>
       <c r="G7">
-        <v>436.1246054499999</v>
+        <v>464.0547980001954</v>
       </c>
       <c r="H7">
-        <v>17.6427</v>
+        <v>17.23163125</v>
       </c>
       <c r="I7">
-        <v>2.998846153846153</v>
+        <v>0.6606009615384559</v>
       </c>
       <c r="J7">
-        <v>16.65949544608248</v>
+        <v>16.50085398043041</v>
       </c>
       <c r="K7">
-        <v>3.689146219116123</v>
+        <v>4.428880971440242</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1909,31 +1909,31 @@
         <v>116</v>
       </c>
       <c r="C8">
-        <v>125.442215</v>
+        <v>128.524949921875</v>
       </c>
       <c r="D8">
-        <v>126.49135</v>
+        <v>129.1841578125</v>
       </c>
       <c r="E8">
-        <v>10.49135</v>
+        <v>13.18415781250002</v>
       </c>
       <c r="F8">
-        <v>10.49135</v>
+        <v>13.18415781250002</v>
       </c>
       <c r="G8">
-        <v>381.7819086787499</v>
+        <v>415.6826678709804</v>
       </c>
       <c r="H8">
-        <v>16.45080833333333</v>
+        <v>16.55705234375</v>
       </c>
       <c r="I8">
-        <v>9.044267241379309</v>
+        <v>11.36565328663795</v>
       </c>
       <c r="J8">
-        <v>15.39029074529862</v>
+        <v>15.64498719813167</v>
       </c>
       <c r="K8">
-        <v>4.594172424151398</v>
+        <v>5.405612043999191</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1944,31 +1944,31 @@
         <v>133</v>
       </c>
       <c r="C9">
-        <v>126.1979935</v>
+        <v>128.7487024257813</v>
       </c>
       <c r="D9">
-        <v>125.442215</v>
+        <v>128.524949921875</v>
       </c>
       <c r="E9">
-        <v>-7.557784999999996</v>
+        <v>-4.47505007812498</v>
       </c>
       <c r="F9">
-        <v>7.557784999999996</v>
+        <v>4.47505007812498</v>
       </c>
       <c r="G9">
-        <v>335.4016523112463</v>
+        <v>359.1602972039441</v>
       </c>
       <c r="H9">
-        <v>15.18037642857143</v>
+        <v>14.83105202008928</v>
       </c>
       <c r="I9">
-        <v>5.682545112781952</v>
+        <v>3.364699306860887</v>
       </c>
       <c r="J9">
-        <v>14.00346994065339</v>
+        <v>13.89066035652156</v>
       </c>
       <c r="K9">
-        <v>4.480789084516869</v>
+        <v>5.732968326805397</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1979,31 +1979,31 @@
         <v>116</v>
       </c>
       <c r="C10">
-        <v>125.17819415</v>
+        <v>128.1112673044922</v>
       </c>
       <c r="D10">
-        <v>126.1979935</v>
+        <v>128.7487024257813</v>
       </c>
       <c r="E10">
-        <v>10.19799350000001</v>
+        <v>12.74870242578126</v>
       </c>
       <c r="F10">
-        <v>10.19799350000001</v>
+        <v>12.74870242578126</v>
       </c>
       <c r="G10">
-        <v>306.4763297005959</v>
+        <v>334.5814367460912</v>
       </c>
       <c r="H10">
-        <v>14.5575785625</v>
+        <v>14.57075832080078</v>
       </c>
       <c r="I10">
-        <v>8.791373706896561</v>
+        <v>10.9902607118804</v>
       </c>
       <c r="J10">
-        <v>13.35195791143378</v>
+        <v>13.52811040094141</v>
       </c>
       <c r="K10">
-        <v>5.373012974938566</v>
+        <v>6.710333927546938</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2014,31 +2014,31 @@
         <v>138</v>
       </c>
       <c r="C11">
-        <v>126.460374735</v>
+        <v>128.6057039392676</v>
       </c>
       <c r="D11">
-        <v>125.17819415</v>
+        <v>128.1112673044922</v>
       </c>
       <c r="E11">
-        <v>-12.82180584999998</v>
+        <v>-9.888732695507798</v>
       </c>
       <c r="F11">
-        <v>12.82180584999998</v>
+        <v>9.888732695507798</v>
       </c>
       <c r="G11">
-        <v>290.689926984429</v>
+        <v>308.2709475879927</v>
       </c>
       <c r="H11">
-        <v>14.36471492777777</v>
+        <v>14.05053325132378</v>
       </c>
       <c r="I11">
-        <v>9.291163659420272</v>
+        <v>7.165748330078115</v>
       </c>
       <c r="J11">
-        <v>12.90075855009895</v>
+        <v>12.8211812819566</v>
       </c>
       <c r="K11">
-        <v>4.552561814055914</v>
+        <v>6.254988308459274</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2049,31 +2049,31 @@
         <v>130</v>
       </c>
       <c r="C12">
-        <v>126.8143372615</v>
+        <v>128.6754187423042</v>
       </c>
       <c r="D12">
-        <v>126.460374735</v>
+        <v>128.6057039392676</v>
       </c>
       <c r="E12">
-        <v>-3.539625264999984</v>
+        <v>-1.394296060732415</v>
       </c>
       <c r="F12">
-        <v>3.539625264999984</v>
+        <v>1.394296060732415</v>
       </c>
       <c r="G12">
-        <v>262.8738289876487</v>
+        <v>277.6382589796909</v>
       </c>
       <c r="H12">
-        <v>13.28220596149999</v>
+        <v>12.78490953226465</v>
       </c>
       <c r="I12">
-        <v>2.722788665384603</v>
+        <v>1.072535431332627</v>
       </c>
       <c r="J12">
-        <v>11.88296156162751</v>
+        <v>11.6463166968942</v>
       </c>
       <c r="K12">
-        <v>4.657104969181974</v>
+        <v>6.765133921021613</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2084,31 +2084,31 @@
         <v>147</v>
       </c>
       <c r="C13">
-        <v>128.83290353535</v>
+        <v>129.591647805189</v>
       </c>
       <c r="D13">
-        <v>126.8143372615</v>
+        <v>128.6754187423042</v>
       </c>
       <c r="E13">
-        <v>-20.18566273849999</v>
+        <v>-18.3245812576958</v>
       </c>
       <c r="F13">
-        <v>20.18566273849999</v>
+        <v>18.3245812576958</v>
       </c>
       <c r="G13">
-        <v>276.018115460814</v>
+        <v>282.9248061878914</v>
       </c>
       <c r="H13">
-        <v>13.90979294122727</v>
+        <v>13.28851605275839</v>
       </c>
       <c r="I13">
-        <v>13.7317433595238</v>
+        <v>12.46570153584748</v>
       </c>
       <c r="J13">
-        <v>12.05103263416354</v>
+        <v>11.72080622770814</v>
       </c>
       <c r="K13">
-        <v>2.995800499875984</v>
+        <v>5.129770971083745</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2119,31 +2119,31 @@
         <v>141</v>
       </c>
       <c r="C14">
-        <v>130.049613181815</v>
+        <v>130.1620654149295</v>
       </c>
       <c r="D14">
-        <v>128.83290353535</v>
+        <v>129.591647805189</v>
       </c>
       <c r="E14">
-        <v>-12.16709646465</v>
+        <v>-11.40835219481102</v>
       </c>
       <c r="F14">
-        <v>12.16709646465</v>
+        <v>11.40835219481102</v>
       </c>
       <c r="G14">
-        <v>265.353125537421</v>
+        <v>270.1936139889712</v>
       </c>
       <c r="H14">
-        <v>13.76456823484583</v>
+        <v>13.13183573126277</v>
       </c>
       <c r="I14">
-        <v>8.629146428829788</v>
+        <v>8.091029925397883</v>
       </c>
       <c r="J14">
-        <v>11.76587545038573</v>
+        <v>11.41832486918228</v>
       </c>
       <c r="K14">
-        <v>2.143464849639037</v>
+        <v>4.322220660001458</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2154,31 +2154,31 @@
         <v>144</v>
       </c>
       <c r="C15">
-        <v>131.4446518636335</v>
+        <v>130.853962144183</v>
       </c>
       <c r="D15">
-        <v>130.049613181815</v>
+        <v>130.1620654149295</v>
       </c>
       <c r="E15">
-        <v>-13.950386818185</v>
+        <v>-13.83793458507046</v>
       </c>
       <c r="F15">
-        <v>13.950386818185</v>
+        <v>13.83793458507046</v>
       </c>
       <c r="G15">
-        <v>259.9115999096956</v>
+        <v>264.1393693421803</v>
       </c>
       <c r="H15">
-        <v>13.77886197202576</v>
+        <v>13.18615102770952</v>
       </c>
       <c r="I15">
-        <v>9.687768623739581</v>
+        <v>9.609676795187818</v>
       </c>
       <c r="J15">
-        <v>11.60602107910525</v>
+        <v>11.27919809425963</v>
       </c>
       <c r="K15">
-        <v>1.128792885453255</v>
+        <v>3.254987526393768</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2189,31 +2189,31 @@
         <v>142</v>
       </c>
       <c r="C16">
-        <v>132.5001866772702</v>
+        <v>131.4112640369739</v>
       </c>
       <c r="D16">
-        <v>131.4446518636335</v>
+        <v>130.853962144183</v>
       </c>
       <c r="E16">
-        <v>-10.55534813636649</v>
+        <v>-11.14603785581696</v>
       </c>
       <c r="F16">
-        <v>10.55534813636649</v>
+        <v>11.14603785581696</v>
       </c>
       <c r="G16">
-        <v>249.3047266504241</v>
+        <v>254.1461400951177</v>
       </c>
       <c r="H16">
-        <v>13.54861098376439</v>
+        <v>13.04042865828862</v>
       </c>
       <c r="I16">
-        <v>7.433343758004571</v>
+        <v>7.849322433673914</v>
       </c>
       <c r="J16">
-        <v>11.30797269902663</v>
+        <v>11.03420697564637</v>
       </c>
       <c r="K16">
-        <v>0.3689037373121107</v>
+        <v>2.436631501398198</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2224,31 +2224,31 @@
         <v>165</v>
       </c>
       <c r="C17">
-        <v>135.7501680095431</v>
+        <v>133.0907008351252</v>
       </c>
       <c r="D17">
-        <v>132.5001866772702</v>
+        <v>131.4112640369739</v>
       </c>
       <c r="E17">
-        <v>-32.49981332272984</v>
+        <v>-33.58873596302612</v>
       </c>
       <c r="F17">
-        <v>32.49981332272984</v>
+        <v>33.58873596302612</v>
       </c>
       <c r="G17">
-        <v>303.1002692745483</v>
+        <v>312.4166096617021</v>
       </c>
       <c r="H17">
-        <v>14.81202447302875</v>
+        <v>14.41031581193779</v>
       </c>
       <c r="I17">
-        <v>19.6968565592302</v>
+        <v>20.35680967456129</v>
       </c>
       <c r="J17">
-        <v>11.8672316230402</v>
+        <v>11.65571382224069</v>
       </c>
       <c r="K17">
-        <v>-1.856713114774359</v>
+        <v>-0.1258832024348464</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2259,51 +2259,51 @@
         <v>173</v>
       </c>
       <c r="C18">
-        <v>139.4751512085888</v>
+        <v>135.0861657933689</v>
       </c>
       <c r="D18">
-        <v>135.7501680095431</v>
+        <v>133.0907008351252</v>
       </c>
       <c r="E18">
-        <v>-37.24983199045687</v>
+        <v>-39.90929916487482</v>
       </c>
       <c r="F18">
-        <v>37.24983199045687</v>
+        <v>39.90929916487482</v>
       </c>
       <c r="G18">
-        <v>370.8783764022181</v>
+        <v>392.4375815473131</v>
       </c>
       <c r="H18">
-        <v>16.21438744286801</v>
+        <v>16.00400227149635</v>
       </c>
       <c r="I18">
-        <v>21.5316947921716</v>
+        <v>23.06895905484094</v>
       </c>
       <c r="J18">
-        <v>12.47126057111092</v>
+        <v>12.36904164927821</v>
       </c>
       <c r="K18">
-        <v>-3.99346027187536</v>
+        <v>-2.607055107814477</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="D19">
-        <v>139.4751512085888</v>
+        <v>135.0861657933689</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="D20">
-        <v>139.4751512085888</v>
+        <v>135.0861657933689</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="D21">
-        <v>139.4751512085888</v>
+        <v>135.0861657933689</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="D22">
-        <v>139.4751512085888</v>
+        <v>135.0861657933689</v>
       </c>
     </row>
   </sheetData>
@@ -2376,10 +2376,10 @@
         <v>98</v>
       </c>
       <c r="C3">
-        <v>103.4</v>
+        <v>103.7</v>
       </c>
       <c r="D3">
-        <v>3.940000000000001</v>
+        <v>3.970000000000001</v>
       </c>
       <c r="E3">
         <v>104</v>
@@ -2414,31 +2414,31 @@
         <v>106</v>
       </c>
       <c r="C4">
-        <v>107.206</v>
+        <v>107.5865</v>
       </c>
       <c r="D4">
-        <v>3.926600000000002</v>
+        <v>3.961650000000001</v>
       </c>
       <c r="E4">
-        <v>107.34</v>
+        <v>107.67</v>
       </c>
       <c r="F4">
-        <v>1.340000000000003</v>
+        <v>1.670000000000002</v>
       </c>
       <c r="G4">
-        <v>1.340000000000003</v>
+        <v>1.670000000000002</v>
       </c>
       <c r="H4">
-        <v>18.8978</v>
+        <v>19.39445</v>
       </c>
       <c r="I4">
-        <v>3.670000000000002</v>
+        <v>3.835000000000001</v>
       </c>
       <c r="J4">
-        <v>1.26415094339623</v>
+        <v>1.575471698113209</v>
       </c>
       <c r="K4">
-        <v>3.693299961494033</v>
+        <v>3.848960338852523</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -2452,31 +2452,31 @@
         <v>109</v>
       </c>
       <c r="C5">
-        <v>110.91934</v>
+        <v>111.4207425</v>
       </c>
       <c r="D5">
-        <v>3.905274000000003</v>
+        <v>3.948909250000001</v>
       </c>
       <c r="E5">
-        <v>111.1326</v>
+        <v>111.54815</v>
       </c>
       <c r="F5">
-        <v>2.132600000000025</v>
+        <v>2.548150000000007</v>
       </c>
       <c r="G5">
-        <v>2.132600000000025</v>
+        <v>2.548150000000007</v>
       </c>
       <c r="H5">
-        <v>14.11452758666671</v>
+        <v>15.09398947416668</v>
       </c>
       <c r="I5">
-        <v>3.157533333333343</v>
+        <v>3.406050000000003</v>
       </c>
       <c r="J5">
-        <v>1.956513761467913</v>
+        <v>2.337752293577988</v>
       </c>
       <c r="K5">
-        <v>3.114371228151993</v>
+        <v>3.345224323761011</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -2490,34 +2490,34 @@
         <v>133</v>
       </c>
       <c r="C6">
-        <v>116.6421526</v>
+        <v>116.2511691625</v>
       </c>
       <c r="D6">
-        <v>4.087027860000003</v>
+        <v>4.037060991250002</v>
       </c>
       <c r="E6">
-        <v>114.824614</v>
+        <v>115.36965175</v>
       </c>
       <c r="F6">
-        <v>-18.17538599999996</v>
+        <v>-17.63034825</v>
       </c>
       <c r="G6">
-        <v>18.17538599999996</v>
+        <v>17.63034825</v>
       </c>
       <c r="H6">
-        <v>93.17205975224867</v>
+        <v>89.0277869596945</v>
       </c>
       <c r="I6">
-        <v>6.911996499999997</v>
+        <v>6.962124562500001</v>
       </c>
       <c r="J6">
-        <v>13.66570375939847</v>
+        <v>13.25590093984962</v>
       </c>
       <c r="K6">
-        <v>5.752204360963612</v>
+        <v>5.822893477783164</v>
       </c>
       <c r="L6">
-        <v>-1.25908426024231</v>
+        <v>-1.064646026289764</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2528,34 +2528,34 @@
         <v>130</v>
       </c>
       <c r="C7">
-        <v>121.656262414</v>
+        <v>120.7738186460625</v>
       </c>
       <c r="D7">
-        <v>4.179736055400004</v>
+        <v>4.08561984048125</v>
       </c>
       <c r="E7">
-        <v>120.72918046</v>
+        <v>120.28823015375</v>
       </c>
       <c r="F7">
-        <v>-9.270819539999962</v>
+        <v>-9.711769846249993</v>
       </c>
       <c r="G7">
-        <v>9.270819539999962</v>
+        <v>9.711769846249993</v>
       </c>
       <c r="H7">
-        <v>91.72726679044796</v>
+        <v>90.08592427706171</v>
       </c>
       <c r="I7">
-        <v>7.38376110799999</v>
+        <v>7.51205361925</v>
       </c>
       <c r="J7">
-        <v>7.131399646153818</v>
+        <v>7.470592189423071</v>
       </c>
       <c r="K7">
-        <v>6.028043418001653</v>
+        <v>6.152433220111145</v>
       </c>
       <c r="L7">
-        <v>-2.43420734732686</v>
+        <v>-2.279532197742704</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2566,34 +2566,34 @@
         <v>116</v>
       </c>
       <c r="C8">
-        <v>124.85239862246</v>
+        <v>124.4164665622166</v>
       </c>
       <c r="D8">
-        <v>4.081376070706004</v>
+        <v>4.041322648048531</v>
       </c>
       <c r="E8">
-        <v>125.8359984694</v>
+        <v>124.8594384865438</v>
       </c>
       <c r="F8">
-        <v>9.835998469400039</v>
+        <v>8.859438486543752</v>
       </c>
       <c r="G8">
-        <v>9.835998469400039</v>
+        <v>8.859438486543752</v>
       </c>
       <c r="H8">
-        <v>92.56386664037996</v>
+        <v>88.15321194702688</v>
       </c>
       <c r="I8">
-        <v>7.792467334899999</v>
+        <v>7.736617763798958</v>
       </c>
       <c r="J8">
-        <v>8.479309025344861</v>
+        <v>7.637446971158407</v>
       </c>
       <c r="K8">
-        <v>6.436587685892188</v>
+        <v>6.399935511952354</v>
       </c>
       <c r="L8">
-        <v>-1.04429145748922</v>
+        <v>-1.068235482484021</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2604,34 +2604,34 @@
         <v>133</v>
       </c>
       <c r="C9">
-        <v>129.3403972238494</v>
+        <v>128.6848997497518</v>
       </c>
       <c r="D9">
-        <v>4.122038323774343</v>
+        <v>4.064033701997205</v>
       </c>
       <c r="E9">
-        <v>128.933774693166</v>
+        <v>128.4577892102651</v>
       </c>
       <c r="F9">
-        <v>-4.066225306833957</v>
+        <v>-4.542210789734924</v>
       </c>
       <c r="G9">
-        <v>4.066225306833957</v>
+        <v>4.542210789734924</v>
       </c>
       <c r="H9">
-        <v>81.70248401260237</v>
+        <v>78.50727864864938</v>
       </c>
       <c r="I9">
-        <v>7.260147045176278</v>
+        <v>7.280273910361239</v>
       </c>
       <c r="J9">
-        <v>3.057312260777411</v>
+        <v>3.415196082507462</v>
       </c>
       <c r="K9">
-        <v>5.953834053732933</v>
+        <v>5.973544164888799</v>
       </c>
       <c r="L9">
-        <v>-1.680934601116953</v>
+        <v>-1.759101451006491</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2642,34 +2642,34 @@
         <v>116</v>
       </c>
       <c r="C10">
-        <v>131.7161919928614</v>
+        <v>131.9114867791616</v>
       </c>
       <c r="D10">
-        <v>3.947413968298106</v>
+        <v>3.980289034738461</v>
       </c>
       <c r="E10">
-        <v>133.4624355476238</v>
+        <v>132.748933451749</v>
       </c>
       <c r="F10">
-        <v>17.46243554762378</v>
+        <v>16.74893345174902</v>
       </c>
       <c r="G10">
-        <v>17.46243554762378</v>
+        <v>16.74893345174902</v>
       </c>
       <c r="H10">
-        <v>109.6067554178914</v>
+        <v>103.7597152889579</v>
       </c>
       <c r="I10">
-        <v>8.535433107982216</v>
+        <v>8.463856353034712</v>
       </c>
       <c r="J10">
-        <v>15.05382374795154</v>
+        <v>14.4387357342664</v>
       </c>
       <c r="K10">
-        <v>7.091332765510259</v>
+        <v>7.031693111060999</v>
       </c>
       <c r="L10">
-        <v>0.6160909591420968</v>
+        <v>0.4657679535043621</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2680,34 +2680,34 @@
         <v>138</v>
       </c>
       <c r="C11">
-        <v>135.8972453650436</v>
+        <v>135.997187023205</v>
       </c>
       <c r="D11">
-        <v>3.970777908686512</v>
+        <v>3.990830155668962</v>
       </c>
       <c r="E11">
-        <v>135.6636059611595</v>
+        <v>135.8917758139</v>
       </c>
       <c r="F11">
-        <v>-2.336394038840496</v>
+        <v>-2.10822418609996</v>
       </c>
       <c r="G11">
-        <v>2.336394038840496</v>
+        <v>2.10822418609996</v>
       </c>
       <c r="H11">
-        <v>98.03475338309562</v>
+        <v>92.72470350339111</v>
       </c>
       <c r="I11">
-        <v>7.846650989188692</v>
+        <v>7.757675001153073</v>
       </c>
       <c r="J11">
-        <v>1.693039158580069</v>
+        <v>1.527698685579681</v>
       </c>
       <c r="K11">
-        <v>6.491522364740238</v>
+        <v>6.420138174896408</v>
       </c>
       <c r="L11">
-        <v>0.3724148219891221</v>
+        <v>0.2364070247767942</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2718,34 +2718,34 @@
         <v>130</v>
       </c>
       <c r="C12">
-        <v>138.8812209463571</v>
+        <v>139.4886163199303</v>
       </c>
       <c r="D12">
-        <v>3.872097675949211</v>
+        <v>3.94089006977459</v>
       </c>
       <c r="E12">
-        <v>139.8680232737301</v>
+        <v>139.988017178874</v>
       </c>
       <c r="F12">
-        <v>9.868023273730074</v>
+        <v>9.988017178874003</v>
       </c>
       <c r="G12">
-        <v>9.868023273730074</v>
+        <v>9.988017178874003</v>
       </c>
       <c r="H12">
-        <v>97.9690663778739</v>
+        <v>93.42828186960023</v>
       </c>
       <c r="I12">
-        <v>8.04878821764283</v>
+        <v>7.980709218925166</v>
       </c>
       <c r="J12">
-        <v>7.590787133638519</v>
+        <v>7.683090137595388</v>
       </c>
       <c r="K12">
-        <v>6.601448841630067</v>
+        <v>6.546433371166306</v>
       </c>
       <c r="L12">
-        <v>1.589087954512648</v>
+        <v>1.481320233676436</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2756,34 +2756,34 @@
         <v>147</v>
       </c>
       <c r="C13">
-        <v>143.1779867600757</v>
+        <v>143.6080310702196</v>
       </c>
       <c r="D13">
-        <v>3.914564489726149</v>
+        <v>3.958742537826065</v>
       </c>
       <c r="E13">
-        <v>142.7533186223063</v>
+        <v>143.4295063897049</v>
       </c>
       <c r="F13">
-        <v>-4.246681377693704</v>
+        <v>-3.570493610295131</v>
       </c>
       <c r="G13">
-        <v>4.246681377693704</v>
+        <v>3.570493610295131</v>
       </c>
       <c r="H13">
-        <v>90.70226968203541</v>
+        <v>86.09374939246915</v>
       </c>
       <c r="I13">
-        <v>7.703142141283819</v>
+        <v>7.579780527231526</v>
       </c>
       <c r="J13">
-        <v>2.888898896390275</v>
+        <v>2.428907217887844</v>
       </c>
       <c r="K13">
-        <v>6.263944301153722</v>
+        <v>6.172112811777354</v>
       </c>
       <c r="L13">
-        <v>1.109099490920463</v>
+        <v>1.088618912532102</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2794,34 +2794,34 @@
         <v>141</v>
       </c>
       <c r="C14">
-        <v>146.4832961248216</v>
+        <v>147.2384349276434</v>
       </c>
       <c r="D14">
-        <v>3.853638977228131</v>
+        <v>3.925908669785835</v>
       </c>
       <c r="E14">
-        <v>147.0925512498018</v>
+        <v>147.5667736080457</v>
       </c>
       <c r="F14">
-        <v>6.092551249801829</v>
+        <v>6.566773608045679</v>
       </c>
       <c r="G14">
-        <v>6.092551249801829</v>
+        <v>6.566773608045679</v>
       </c>
       <c r="H14">
-        <v>86.23701226948761</v>
+        <v>82.51281324470715</v>
       </c>
       <c r="I14">
-        <v>7.56892623366032</v>
+        <v>7.495363283966039</v>
       </c>
       <c r="J14">
-        <v>4.320958333192787</v>
+        <v>4.657286246840908</v>
       </c>
       <c r="K14">
-        <v>6.102028803823644</v>
+        <v>6.045877264699318</v>
       </c>
       <c r="L14">
-        <v>1.93370919802315</v>
+        <v>1.9769910385173</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2832,34 +2832,34 @@
         <v>144</v>
       </c>
       <c r="C15">
-        <v>149.7032415918448</v>
+        <v>150.8061264175577</v>
       </c>
       <c r="D15">
-        <v>3.790269626207635</v>
+        <v>3.890086951798687</v>
       </c>
       <c r="E15">
-        <v>150.3369351020498</v>
+        <v>151.1643435974292</v>
       </c>
       <c r="F15">
-        <v>6.336935102049779</v>
+        <v>7.164343597429223</v>
       </c>
       <c r="G15">
-        <v>6.336935102049779</v>
+        <v>7.164343597429223</v>
       </c>
       <c r="H15">
-        <v>82.69237644011092</v>
+        <v>80.11396754757776</v>
       </c>
       <c r="I15">
-        <v>7.474157685074894</v>
+        <v>7.469900231155515</v>
       </c>
       <c r="J15">
-        <v>4.400649376423457</v>
+        <v>4.975238609325849</v>
       </c>
       <c r="K15">
-        <v>5.971153463254399</v>
+        <v>5.963520445055204</v>
       </c>
       <c r="L15">
-        <v>2.80607370929816</v>
+        <v>2.942825065932802</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2870,34 +2870,34 @@
         <v>142</v>
       </c>
       <c r="C16">
-        <v>152.3441600962472</v>
+        <v>154.0614027008886</v>
       </c>
       <c r="D16">
-        <v>3.675334514027112</v>
+        <v>3.826605884951904</v>
       </c>
       <c r="E16">
-        <v>153.4935112180524</v>
+        <v>154.6962133693564</v>
       </c>
       <c r="F16">
-        <v>11.49351121805245</v>
+        <v>12.69621336935643</v>
       </c>
       <c r="G16">
-        <v>11.49351121805245</v>
+        <v>12.69621336935643</v>
       </c>
       <c r="H16">
-        <v>86.22154956006712</v>
+        <v>85.90538657419542</v>
       </c>
       <c r="I16">
-        <v>7.761254366001862</v>
+        <v>7.84320831245558</v>
       </c>
       <c r="J16">
-        <v>8.094021984543977</v>
+        <v>8.940995330532695</v>
       </c>
       <c r="K16">
-        <v>6.122786929060797</v>
+        <v>6.176197222589311</v>
       </c>
       <c r="L16">
-        <v>4.183157395215581</v>
+        <v>4.421509875562739</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2908,34 +2908,34 @@
         <v>165</v>
       </c>
       <c r="C17">
-        <v>156.9175451492469</v>
+        <v>158.2436081565485</v>
       </c>
       <c r="D17">
-        <v>3.765139567924368</v>
+        <v>3.862165842022701</v>
       </c>
       <c r="E17">
-        <v>156.0194946102743</v>
+        <v>157.8880085858405</v>
       </c>
       <c r="F17">
-        <v>-8.980505389725693</v>
+        <v>-7.11199141415949</v>
       </c>
       <c r="G17">
-        <v>8.980505389725693</v>
+        <v>7.11199141415949</v>
       </c>
       <c r="H17">
-        <v>85.85007805972212</v>
+        <v>83.55038892758762</v>
       </c>
       <c r="I17">
-        <v>7.84253776758345</v>
+        <v>7.794460519235841</v>
       </c>
       <c r="J17">
-        <v>5.442730539227692</v>
+        <v>4.310297826763327</v>
       </c>
       <c r="K17">
-        <v>6.077449836405257</v>
+        <v>6.051803929534246</v>
       </c>
       <c r="L17">
-        <v>2.99469940771494</v>
+        <v>3.53672092217631</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2946,54 +2946,54 @@
         <v>173</v>
       </c>
       <c r="C18">
-        <v>161.9144162454541</v>
+        <v>162.6504852986426</v>
       </c>
       <c r="D18">
-        <v>3.888312720752657</v>
+        <v>3.916636972029846</v>
       </c>
       <c r="E18">
-        <v>160.6826847171712</v>
+        <v>162.1057739985712</v>
       </c>
       <c r="F18">
-        <v>-12.31731528282876</v>
+        <v>-10.89422600142882</v>
       </c>
       <c r="G18">
-        <v>12.31731528282876</v>
+        <v>10.89422600142882</v>
       </c>
       <c r="H18">
-        <v>89.96671416702742</v>
+        <v>85.74624963025137</v>
       </c>
       <c r="I18">
-        <v>8.122211362286283</v>
+        <v>7.988195861872902</v>
       </c>
       <c r="J18">
-        <v>7.119835423600438</v>
+        <v>6.297240463253654</v>
       </c>
       <c r="K18">
-        <v>6.142598935604956</v>
+        <v>6.067143712891708</v>
       </c>
       <c r="L18">
-        <v>1.375084620008167</v>
+        <v>2.087155332984132</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="E19">
-        <v>164.5709974379239</v>
+        <v>166.022410970601</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="E20">
-        <v>172.3476228794292</v>
+        <v>173.8556849146607</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="E21">
-        <v>184.0125610416872</v>
+        <v>185.6055958307502</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="E22">
-        <v>199.5658119246978</v>
+        <v>201.2721437188696</v>
       </c>
     </row>
   </sheetData>
@@ -3069,13 +3069,13 @@
         <v>98</v>
       </c>
       <c r="C3">
-        <v>108.7856364997036</v>
+        <v>109.2407900263829</v>
       </c>
       <c r="D3">
-        <v>2.875737309644022</v>
+        <v>2.949699757729399</v>
       </c>
       <c r="E3">
-        <v>0.9861455576906619</v>
+        <v>0.990696294007365</v>
       </c>
       <c r="F3">
         <v>109.3290258543759</v>
@@ -3110,37 +3110,37 @@
         <v>106</v>
       </c>
       <c r="C4">
-        <v>111.7132263929941</v>
+        <v>112.1928409762887</v>
       </c>
       <c r="D4">
-        <v>2.88092256800867</v>
+        <v>2.949817317338223</v>
       </c>
       <c r="E4">
-        <v>0.9448690013829411</v>
+        <v>0.9444445703936377</v>
       </c>
       <c r="F4">
-        <v>105.4558787096639</v>
+        <v>105.9555894704629</v>
       </c>
       <c r="G4">
-        <v>-0.5441212903360508</v>
+        <v>-0.04441052953711733</v>
       </c>
       <c r="H4">
-        <v>0.5441212903360508</v>
+        <v>0.04441052953711733</v>
       </c>
       <c r="I4">
-        <v>64.32144739385711</v>
+        <v>64.17439955212551</v>
       </c>
       <c r="J4">
-        <v>5.936573572355968</v>
+        <v>5.686718191956501</v>
       </c>
       <c r="K4">
-        <v>0.5133219720151423</v>
+        <v>0.04189672597841257</v>
       </c>
       <c r="L4">
-        <v>6.036776217832002</v>
+        <v>5.801063594813638</v>
       </c>
       <c r="M4">
-        <v>1.816688436956366</v>
+        <v>1.984380963487892</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3151,37 +3151,37 @@
         <v>109</v>
       </c>
       <c r="C5">
-        <v>113.7925059591224</v>
+        <v>114.6698756037288</v>
       </c>
       <c r="D5">
-        <v>2.800758267820626</v>
+        <v>2.926178182843317</v>
       </c>
       <c r="E5">
-        <v>1.024000894415179</v>
+        <v>1.027307614197757</v>
       </c>
       <c r="F5">
-        <v>118.1863588276995</v>
+        <v>118.7520624119892</v>
       </c>
       <c r="G5">
-        <v>9.186358827699536</v>
+        <v>9.752062411989186</v>
       </c>
       <c r="H5">
-        <v>9.186358827699536</v>
+        <v>9.752062411989186</v>
       </c>
       <c r="I5">
-        <v>71.01069443298914</v>
+        <v>74.48384013052778</v>
       </c>
       <c r="J5">
-        <v>7.019835324137158</v>
+        <v>7.041832931967396</v>
       </c>
       <c r="K5">
-        <v>8.427852135504162</v>
+        <v>8.946846249531363</v>
       </c>
       <c r="L5">
-        <v>6.833801523722722</v>
+        <v>6.849657813052879</v>
       </c>
       <c r="M5">
-        <v>2.844976052795674</v>
+        <v>2.9873866562964</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3192,37 +3192,37 @@
         <v>133</v>
       </c>
       <c r="C6">
-        <v>117.7304273612062</v>
+        <v>118.1776716054036</v>
       </c>
       <c r="D6">
-        <v>2.914474581246947</v>
+        <v>2.955259073784887</v>
       </c>
       <c r="E6">
-        <v>1.039236854531764</v>
+        <v>1.033997386545341</v>
       </c>
       <c r="F6">
-        <v>119.9960915916242</v>
+        <v>121.0281480199456</v>
       </c>
       <c r="G6">
-        <v>-13.00390840837579</v>
+        <v>-11.97185198005444</v>
       </c>
       <c r="H6">
-        <v>13.00390840837579</v>
+        <v>11.97185198005444</v>
       </c>
       <c r="I6">
-        <v>95.53342929809853</v>
+        <v>91.69419005597919</v>
       </c>
       <c r="J6">
-        <v>8.515853595196816</v>
+        <v>8.274337693989157</v>
       </c>
       <c r="K6">
-        <v>9.777374743139694</v>
+        <v>9.001392466206344</v>
       </c>
       <c r="L6">
-        <v>7.569694828576965</v>
+        <v>7.387591476341245</v>
       </c>
       <c r="M6">
-        <v>0.8181628424534405</v>
+        <v>1.09553490466779</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3233,37 +3233,37 @@
         <v>130</v>
       </c>
       <c r="C7">
-        <v>121.6512350567574</v>
+        <v>121.6373261510566</v>
       </c>
       <c r="D7">
-        <v>3.015107892677377</v>
+        <v>2.980478847378293</v>
       </c>
       <c r="E7">
-        <v>0.9943938709581061</v>
+        <v>0.9945990235681055</v>
       </c>
       <c r="F7">
-        <v>118.9734341085757</v>
+        <v>120.0059455061231</v>
       </c>
       <c r="G7">
-        <v>-11.02656589142433</v>
+        <v>-9.994054493876945</v>
       </c>
       <c r="H7">
-        <v>11.02656589142433</v>
+        <v>9.994054493876945</v>
       </c>
       <c r="I7">
-        <v>100.7437745100633</v>
+        <v>93.33157709009974</v>
       </c>
       <c r="J7">
-        <v>9.017996054442317</v>
+        <v>8.618281053966715</v>
       </c>
       <c r="K7">
-        <v>8.481973762634096</v>
+        <v>7.687734226059188</v>
       </c>
       <c r="L7">
-        <v>7.752150615388392</v>
+        <v>7.447620026284834</v>
       </c>
       <c r="M7">
-        <v>-0.4501233847913648</v>
+        <v>-0.1078206583522517</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3274,37 +3274,37 @@
         <v>116</v>
       </c>
       <c r="C8">
-        <v>124.495522796645</v>
+        <v>124.5280904001267</v>
       </c>
       <c r="D8">
-        <v>2.998025877398394</v>
+        <v>2.975993117462882</v>
       </c>
       <c r="E8">
-        <v>0.9435581427553752</v>
+        <v>0.9437981785495505</v>
       </c>
       <c r="F8">
-        <v>117.7933629686957</v>
+        <v>117.694609305145</v>
       </c>
       <c r="G8">
-        <v>1.793362968695732</v>
+        <v>1.694609305144951</v>
       </c>
       <c r="H8">
-        <v>1.793362968695732</v>
+        <v>1.694609305144951</v>
       </c>
       <c r="I8">
-        <v>84.4891705479676</v>
+        <v>78.2549310245971</v>
       </c>
       <c r="J8">
-        <v>7.81389054015122</v>
+        <v>7.464335762496421</v>
       </c>
       <c r="K8">
-        <v>1.546002559220458</v>
+        <v>1.460870090642199</v>
       </c>
       <c r="L8">
-        <v>6.717792606027071</v>
+        <v>6.449828370344394</v>
       </c>
       <c r="M8">
-        <v>-0.289976923495676</v>
+        <v>0.1025383359477311</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -3315,37 +3315,37 @@
         <v>133</v>
       </c>
       <c r="C9">
-        <v>127.7085722082084</v>
+        <v>127.602110833519</v>
       </c>
       <c r="D9">
-        <v>3.019528230814897</v>
+        <v>2.980894483259353</v>
       </c>
       <c r="E9">
-        <v>1.025744166456996</v>
+        <v>1.028057358829927</v>
       </c>
       <c r="F9">
-        <v>130.5535078743856</v>
+        <v>130.9859158389264</v>
       </c>
       <c r="G9">
-        <v>-2.446492125614384</v>
+        <v>-2.014084161073555</v>
       </c>
       <c r="H9">
-        <v>2.446492125614384</v>
+        <v>2.014084161073555</v>
       </c>
       <c r="I9">
-        <v>73.27433528692839</v>
+        <v>67.65516016506713</v>
       </c>
       <c r="J9">
-        <v>7.04711933807453</v>
+        <v>6.685728390864583</v>
       </c>
       <c r="K9">
-        <v>1.839467763619838</v>
+        <v>1.514348993288387</v>
       </c>
       <c r="L9">
-        <v>6.020889057111751</v>
+        <v>5.744759887907821</v>
       </c>
       <c r="M9">
-        <v>-0.6686902603620367</v>
+        <v>-0.186771510900483</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3356,37 +3356,37 @@
         <v>116</v>
       </c>
       <c r="C10">
-        <v>129.0084045072139</v>
+        <v>129.6631535612366</v>
       </c>
       <c r="D10">
-        <v>2.847558637633959</v>
+        <v>2.934901895482268</v>
       </c>
       <c r="E10">
-        <v>1.025229791521208</v>
+        <v>1.027028806259727</v>
       </c>
       <c r="F10">
-        <v>135.8574598991631</v>
+        <v>135.0224862247852</v>
       </c>
       <c r="G10">
-        <v>19.85745989916308</v>
+        <v>19.02248622478515</v>
       </c>
       <c r="H10">
-        <v>19.85745989916308</v>
+        <v>19.02248622478515</v>
       </c>
       <c r="I10">
-        <v>113.4048825819211</v>
+        <v>104.4301379159514</v>
       </c>
       <c r="J10">
-        <v>8.648411908210598</v>
+        <v>8.227823120104654</v>
       </c>
       <c r="K10">
-        <v>17.11849991307162</v>
+        <v>16.39869502136651</v>
       </c>
       <c r="L10">
-        <v>7.408090414106733</v>
+        <v>7.076501779590159</v>
       </c>
       <c r="M10">
-        <v>1.751202416689387</v>
+        <v>2.160204755535271</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -3397,37 +3397,37 @@
         <v>138</v>
       </c>
       <c r="C11">
-        <v>132.4789471294101</v>
+        <v>132.9056217910276</v>
       </c>
       <c r="D11">
-        <v>2.909857036090178</v>
+        <v>2.950280212197705</v>
       </c>
       <c r="E11">
-        <v>0.9991219783889517</v>
+        <v>0.996785612164437</v>
       </c>
       <c r="F11">
-        <v>131.1167616005146</v>
+        <v>131.8818964842821</v>
       </c>
       <c r="G11">
-        <v>-6.88323839948535</v>
+        <v>-6.118103515717905</v>
       </c>
       <c r="H11">
-        <v>6.88323839948535</v>
+        <v>6.118103515717905</v>
       </c>
       <c r="I11">
-        <v>106.0686701688354</v>
+        <v>96.98581043962785</v>
       </c>
       <c r="J11">
-        <v>8.452281518352237</v>
+        <v>7.993409830728349</v>
       </c>
       <c r="K11">
-        <v>4.987853912670544</v>
+        <v>4.43340834472312</v>
       </c>
       <c r="L11">
-        <v>7.139175247280489</v>
+        <v>6.782824731271599</v>
       </c>
       <c r="M11">
-        <v>0.9774735279178171</v>
+        <v>1.45816108054767</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3438,37 +3438,37 @@
         <v>130</v>
       </c>
       <c r="C12">
-        <v>135.6036835842328</v>
+        <v>135.9501725360888</v>
       </c>
       <c r="D12">
-        <v>2.931344977963434</v>
+        <v>2.954993738840879</v>
       </c>
       <c r="E12">
-        <v>0.9450699307188639</v>
+        <v>0.9444199044199216</v>
       </c>
       <c r="F12">
-        <v>127.7472086082706</v>
+        <v>128.2205528558503</v>
       </c>
       <c r="G12">
-        <v>-2.252791391729374</v>
+        <v>-1.779447144149714</v>
       </c>
       <c r="H12">
-        <v>2.252791391729374</v>
+        <v>1.779447144149714</v>
       </c>
       <c r="I12">
-        <v>95.96931005741681</v>
+        <v>87.60387260954732</v>
       </c>
       <c r="J12">
-        <v>7.83233250568995</v>
+        <v>7.372013562070485</v>
       </c>
       <c r="K12">
-        <v>1.732916455176442</v>
+        <v>1.36880549549978</v>
       </c>
       <c r="L12">
-        <v>6.598549368070084</v>
+        <v>6.241422807694417</v>
       </c>
       <c r="M12">
-        <v>0.7672159013427391</v>
+        <v>1.339692593988078</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -3479,37 +3479,37 @@
         <v>147</v>
       </c>
       <c r="C13">
-        <v>138.9648289438416</v>
+        <v>139.109314496598</v>
       </c>
       <c r="D13">
-        <v>2.974325016127965</v>
+        <v>2.965201149924297</v>
       </c>
       <c r="E13">
-        <v>1.028951911468478</v>
+        <v>1.029490636523953</v>
       </c>
       <c r="F13">
-        <v>142.1014973976262</v>
+        <v>142.802478368436</v>
       </c>
       <c r="G13">
-        <v>-4.898502602373838</v>
+        <v>-4.197521631564001</v>
       </c>
       <c r="H13">
-        <v>4.898502602373838</v>
+        <v>4.197521631564001</v>
       </c>
       <c r="I13">
-        <v>89.42622075633011</v>
+        <v>81.24162854026554</v>
       </c>
       <c r="J13">
-        <v>7.565620696297577</v>
+        <v>7.083423386569896</v>
       </c>
       <c r="K13">
-        <v>3.332314695492407</v>
+        <v>2.855456892220409</v>
       </c>
       <c r="L13">
-        <v>6.301618943290296</v>
+        <v>5.933607724469507</v>
       </c>
       <c r="M13">
-        <v>0.1467939624753597</v>
+        <v>0.8016900911342223</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -3520,37 +3520,37 @@
         <v>141</v>
       </c>
       <c r="C14">
-        <v>141.5423429879891</v>
+        <v>141.8352516563391</v>
       </c>
       <c r="D14">
-        <v>2.934643918929919</v>
+        <v>2.953237950415132</v>
       </c>
       <c r="E14">
-        <v>1.022323645765695</v>
+        <v>1.025382921636675</v>
       </c>
       <c r="F14">
-        <v>145.5202492230762</v>
+        <v>145.9146202043768</v>
       </c>
       <c r="G14">
-        <v>4.520249223076178</v>
+        <v>4.914620204376803</v>
       </c>
       <c r="H14">
-        <v>4.520249223076178</v>
+        <v>4.914620204376803</v>
       </c>
       <c r="I14">
-        <v>83.67675677986267</v>
+        <v>76.4842838080158</v>
       </c>
       <c r="J14">
-        <v>7.311839740195794</v>
+        <v>6.902689788053805</v>
       </c>
       <c r="K14">
-        <v>3.205850512819984</v>
+        <v>3.485546244238867</v>
       </c>
       <c r="L14">
-        <v>6.043638240751103</v>
+        <v>5.729602601116953</v>
       </c>
       <c r="M14">
-        <v>0.7700984791442528</v>
+        <v>1.534667045740884</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -3561,37 +3561,37 @@
         <v>144</v>
       </c>
       <c r="C15">
-        <v>144.4454472453041</v>
+        <v>144.7722833512119</v>
       </c>
       <c r="D15">
-        <v>2.931489952768429</v>
+        <v>2.952427637638018</v>
       </c>
       <c r="E15">
-        <v>0.998901396136564</v>
+        <v>0.9966796080738831</v>
       </c>
       <c r="F15">
-        <v>144.3501329901156</v>
+        <v>144.3230832470327</v>
       </c>
       <c r="G15">
-        <v>0.3501329901155543</v>
+        <v>0.323083247032713</v>
       </c>
       <c r="H15">
-        <v>0.3501329901155543</v>
+        <v>0.323083247032713</v>
       </c>
       <c r="I15">
-        <v>77.24951342070149</v>
+        <v>70.6089068062079</v>
       </c>
       <c r="J15">
-        <v>6.776323836343467</v>
+        <v>6.396566207975259</v>
       </c>
       <c r="K15">
-        <v>0.2431479098024683</v>
+        <v>0.2243633659949396</v>
       </c>
       <c r="L15">
-        <v>5.597446676831978</v>
+        <v>5.30612265995372</v>
       </c>
       <c r="M15">
-        <v>0.8826274833131647</v>
+        <v>1.706605299906127</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -3602,37 +3602,37 @@
         <v>142</v>
       </c>
       <c r="C16">
-        <v>147.6358216759156</v>
+        <v>147.8563178385052</v>
       </c>
       <c r="D16">
-        <v>2.957378400552735</v>
+        <v>2.959007980120784</v>
       </c>
       <c r="E16">
-        <v>0.9467455567349878</v>
+        <v>0.9452185008118785</v>
       </c>
       <c r="F16">
-        <v>139.2815118273408</v>
+        <v>139.5141574325502</v>
       </c>
       <c r="G16">
-        <v>-2.718488172659249</v>
+        <v>-2.485842567449822</v>
       </c>
       <c r="H16">
-        <v>2.718488172659249</v>
+        <v>2.485842567449822</v>
       </c>
       <c r="I16">
-        <v>72.25956088671482</v>
+        <v>66.00680012506059</v>
       </c>
       <c r="J16">
-        <v>6.486478431794595</v>
+        <v>6.117228805080585</v>
       </c>
       <c r="K16">
-        <v>1.914428290605105</v>
+        <v>1.75059335735903</v>
       </c>
       <c r="L16">
-        <v>5.334373934958629</v>
+        <v>5.052156281196957</v>
       </c>
       <c r="M16">
-        <v>0.5029665195733909</v>
+        <v>1.378168365597065</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -3643,37 +3643,37 @@
         <v>165</v>
       </c>
       <c r="C17">
-        <v>151.4719734120989</v>
+        <v>151.2882312477755</v>
       </c>
       <c r="D17">
-        <v>3.0452557341158</v>
+        <v>2.98265325157826</v>
       </c>
       <c r="E17">
-        <v>1.03498776299782</v>
+        <v>1.032547775350236</v>
       </c>
       <c r="F17">
-        <v>154.953161072837</v>
+        <v>155.2629657745847</v>
       </c>
       <c r="G17">
-        <v>-10.04683892716301</v>
+        <v>-9.7370342254153</v>
       </c>
       <c r="H17">
-        <v>10.04683892716301</v>
+        <v>9.7370342254153</v>
       </c>
       <c r="I17">
-        <v>74.17152165615771</v>
+        <v>67.92700248385049</v>
       </c>
       <c r="J17">
-        <v>6.723835798152489</v>
+        <v>6.358549166436233</v>
       </c>
       <c r="K17">
-        <v>6.088993289189702</v>
+        <v>5.90123286388806</v>
       </c>
       <c r="L17">
-        <v>5.384681891907367</v>
+        <v>5.108761386709697</v>
       </c>
       <c r="M17">
-        <v>-1.009001059767039</v>
+        <v>-0.2054655813672566</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -3684,37 +3684,37 @@
         <v>173</v>
       </c>
       <c r="C18">
-        <v>155.8406891605757</v>
+        <v>154.9932131736472</v>
       </c>
       <c r="D18">
-        <v>3.177601735551892</v>
+        <v>3.01876968529293</v>
       </c>
       <c r="E18">
-        <v>1.03110208390814</v>
+        <v>1.029922670814719</v>
       </c>
       <c r="F18">
-        <v>157.9666170343716</v>
+        <v>158.1867302714215</v>
       </c>
       <c r="G18">
-        <v>-15.03338296562845</v>
+        <v>-14.81326972857852</v>
       </c>
       <c r="H18">
-        <v>15.03338296562845</v>
+        <v>14.81326972857852</v>
       </c>
       <c r="I18">
-        <v>83.66096426460081</v>
+        <v>77.39612483183613</v>
       </c>
       <c r="J18">
-        <v>7.243182496119736</v>
+        <v>6.886969201570126</v>
       </c>
       <c r="K18">
-        <v>8.689816743137831</v>
+        <v>8.562583658137871</v>
       </c>
       <c r="L18">
-        <v>5.591252820109272</v>
+        <v>5.324625278673959</v>
       </c>
       <c r="M18">
-        <v>-3.012175990781939</v>
+        <v>-2.340613448080698</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -3722,10 +3722,10 @@
         <v>17</v>
       </c>
       <c r="E19">
-        <v>0.998901396136564</v>
+        <v>0.9966796080738831</v>
       </c>
       <c r="F19">
-        <v>151.3055657169062</v>
+        <v>150.7858950262239</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -3733,10 +3733,10 @@
         <v>18</v>
       </c>
       <c r="E20">
-        <v>0.9467455567349878</v>
+        <v>0.9452185008118785</v>
       </c>
       <c r="F20">
-        <v>146.2885001331808</v>
+        <v>145.8196941654017</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -3744,10 +3744,10 @@
         <v>19</v>
       </c>
       <c r="E21">
-        <v>1.03498776299782</v>
+        <v>1.032547775350236</v>
       </c>
       <c r="F21">
-        <v>163.0752437586711</v>
+        <v>162.3717905706792</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -3755,10 +3755,10 @@
         <v>20</v>
       </c>
       <c r="E22">
-        <v>1.03110208390814</v>
+        <v>1.029922670814719</v>
       </c>
       <c r="F22">
-        <v>165.6029760393337</v>
+        <v>165.0308857984829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>